<commit_message>
all cols in place for final output
</commit_message>
<xml_diff>
--- a/INPUT-FILES/OES-INPUT-TABLES/TOD-S/TODS CI.xlsx
+++ b/INPUT-FILES/OES-INPUT-TABLES/TOD-S/TODS CI.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpspublish1-my.sharepoint.com/personal/aklein_wpspublish_com/Documents/Desktop/TOD/OES/input files for TOD S/input score files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wpspublish1-my.sharepoint.com/personal/dherzberg_wpspublish_com/Documents/Desktop/R/TOD-R/INPUT-FILES/OES-INPUT-TABLES/TOD-S/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C8E7FAEE-7FCC-452C-8CB6-0FAC7689FE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97B77B2C-C3AC-44B6-B25C-1329F18C6BDB}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{C8E7FAEE-7FCC-452C-8CB6-0FAC7689FE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E3F0BED-C53E-924C-869B-DB0059204BB4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{217BF118-6C1C-42C8-9F8C-396830CB1CD1}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{217BF118-6C1C-42C8-9F8C-396830CB1CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CV90" sheetId="2" r:id="rId2"/>
+    <sheet name="CV95" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="41">
   <si>
     <t>grade K-1; ages 5-6</t>
   </si>
@@ -84,15 +86,97 @@
   </si>
   <si>
     <t>LWC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &amp; test == </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">age_grade %in% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c(age_low, grade_low) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"PV" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"LWC" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c(age_middle, grade_middle) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c(age_high, grade_high) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"WRF" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"QRF" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">test == </t>
+  </si>
+  <si>
+    <t xml:space="preserve">norm_group %in% </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("age", "grade") </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"DRIW" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">"DRIQ" </t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("adult") </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp; test == </t>
+  </si>
+  <si>
+    <t xml:space="preserve">~ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -119,8 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,7 +514,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,16 +524,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA4CA78-A576-4181-B554-47B34E2C6277}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="179" workbookViewId="0">
+      <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -460,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -474,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -485,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -499,7 +586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>15</v>
       </c>
@@ -510,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -524,7 +611,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -535,7 +622,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -549,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -563,7 +650,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -577,7 +664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>11</v>
       </c>
@@ -588,7 +675,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -601,6 +688,595 @@
       <c r="D18">
         <v>9</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B89B3F-0751-2A47-A294-81992A84CB17}">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="6:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCC3FA6-E7B9-D447-91E6-C3ADD58C190B}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="1">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="1">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="1">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="1">
+        <v>9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="6:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>